<commit_message>
trait import: add check for nominal label
</commit_message>
<xml_diff>
--- a/src/test/resources/files/ontology/data_ordinal_missing_categories.xlsx
+++ b/src/test/resources/files/ontology/data_ordinal_missing_categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ct447/Documents/projects/bi-api/src/test/resources/files/ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C94E161-263D-6149-ABD8-E74AA1A94CC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B72F13-5214-AB4D-B7B6-44BBC890963D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="7060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,7 +180,7 @@
     <t>CrType 1-2 scale</t>
   </si>
   <si>
-    <t>FEW=1; MANY=2</t>
+    <t>1;2</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -818,18 +818,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1011,14 +1011,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7613A94-47D1-485D-A76D-D3A6CFAB63B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EFE1791-BEC8-419B-A7D8-F7EAC9E3F094}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -1030,6 +1022,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7613A94-47D1-485D-A76D-D3A6CFAB63B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[BI-1613] - Even more unit test updates
</commit_message>
<xml_diff>
--- a/src/test/resources/files/ontology/data_ordinal_missing_categories.xlsx
+++ b/src/test/resources/files/ontology/data_ordinal_missing_categories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hms243/IdeaProjects/bi-api/src/test/resources/files/ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DC5CE5-2545-CC43-98BD-357EEC9EDA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56454040-2B8D-634A-868F-5FFAA98ED29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8160" yWindow="3880" windowWidth="25020" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6100" windowWidth="25020" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>ALFALFA SNOUT BEETLE</t>
   </si>
@@ -184,18 +184,6 @@
   </si>
   <si>
     <t>Term Type</t>
-  </si>
-  <si>
-    <t>Phenotype</t>
-  </si>
-  <si>
-    <t>Germplasm Attribute</t>
-  </si>
-  <si>
-    <t>phenotype</t>
-  </si>
-  <si>
-    <t>germplasm passport</t>
   </si>
 </sst>
 </file>
@@ -301,7 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -312,8 +300,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -716,9 +703,7 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>53</v>
-      </c>
+      <c r="C3" s="8"/>
       <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
@@ -749,9 +734,7 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>54</v>
-      </c>
+      <c r="C4" s="8"/>
       <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
@@ -782,9 +765,7 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>55</v>
-      </c>
+      <c r="C5" s="8"/>
       <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
@@ -815,9 +796,7 @@
       <c r="B6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="C6" s="8"/>
       <c r="D6" s="6" t="s">
         <v>46</v>
       </c>
@@ -842,15 +821,6 @@
       <c r="R6" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C8" s="9"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C9" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -859,21 +829,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006D74C1D9EC8A1042A5EF45985DF3E9E4" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2000d971e1751a7db8d92151125d08a9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="aa5be1c8-7296-4b7a-853c-c6802fcefdea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a4a1f299a0d30015388c519f6ad441cc" ns3:_="">
     <xsd:import namespace="aa5be1c8-7296-4b7a-853c-c6802fcefdea"/>
@@ -1051,10 +1006,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7613A94-47D1-485D-A76D-D3A6CFAB63B4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{340A8394-9E0A-435F-BF61-25A36768AA02}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="aa5be1c8-7296-4b7a-853c-c6802fcefdea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1076,19 +1056,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{340A8394-9E0A-435F-BF61-25A36768AA02}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7613A94-47D1-485D-A76D-D3A6CFAB63B4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="aa5be1c8-7296-4b7a-853c-c6802fcefdea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>